<commit_message>
Footer y arreglar cosas
</commit_message>
<xml_diff>
--- a/Result_df/df_posts.xlsx
+++ b/Result_df/df_posts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +441,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Likes</t>
+          <t>Label</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Label</t>
+          <t>Rate</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Rate</t>
+          <t>Id</t>
         </is>
       </c>
     </row>
@@ -461,19 +461,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AT_USER hola noeee</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>Tocara ir a ver saww</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>-1.137231677157825</v>
       </c>
       <c r="E2" t="n">
-        <v>1.790779697604845</v>
+        <v>1.396257002800693e+18</v>
       </c>
     </row>
     <row r="3">
@@ -482,19 +482,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AT_USER Hola AT_USER me gustaría ver a AT_USER con una nominación o perfomance #PremiosMTVMiaw, gracias!!</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>De lo cos</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-1.653342728774344</v>
       </c>
       <c r="E3" t="n">
-        <v>4.840540904667252</v>
+        <v>1.396230674542121e+18</v>
       </c>
     </row>
     <row r="4">
@@ -503,20 +503,19 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola AT_USER nos encantaria ver como Host, o nominado o presentando su single a AT_USER 
-JOAQUIN EN LOS MTVMIAW</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
+          <t>AT_USER JAJAJAJAJAJAJAJAJAJAJAJAJAAJAJAJAJAJAJAJAJAJAJAJAJAJA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.03471381228373671</v>
+        <v>1.394666359141847e+18</v>
       </c>
     </row>
     <row r="5">
@@ -525,19 +524,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AT_USER Hola</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>Regalando dinero a la urban🤑</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>-1.02473406935197</v>
       </c>
       <c r="E5" t="n">
-        <v>1.790779697604845</v>
+        <v>1.393950120664879e+18</v>
       </c>
     </row>
     <row r="6">
@@ -546,19 +545,19 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola buenas, quisiera volver al pasado y cambiar algunas cosas, ahora seria mas feliz...</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
+          <t>AT_USER 🌚👌🏻</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.7809568132404325</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1534888459190395</v>
+        <v>1.393305669688775e+18</v>
       </c>
     </row>
     <row r="7">
@@ -567,20 +566,19 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola AT_USER nos encantaria ver como Host, o nominado o presentando su single a AT_USER 
-JOAQUIN EN LOS MTVMI…</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>He convertido a mi hermana en una posadora fitness 💁🏻‍♂️</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.7509834102645365</v>
       </c>
       <c r="E7" t="n">
-        <v>0.614528551935965</v>
+        <v>1.393300041851408e+18</v>
       </c>
     </row>
     <row r="8">
@@ -589,20 +587,19 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>RT AT_USER no tengo mucho tiempo para andar activo en tw pero bueno hola
-I just voted for AT_USER for #BBMAsTopSocial</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>AT_USER AT_USER Soy yo capullo 🥲</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>1.115841535356569</v>
+        <v>1.392957179645334e+18</v>
       </c>
     </row>
     <row r="9">
@@ -611,19 +608,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>AT_USER hola maria, amor de mi vida, luz de mis ojos</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>AT_USER AT_USER</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>3.224598344677971</v>
+        <v>1.392953588486484e+18</v>
       </c>
     </row>
     <row r="10">
@@ -632,19 +629,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola, AT_USER  eres mudo verdad? 😂😍 #24LunasSinTi</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>Chiklin</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>1.569438672299835</v>
+        <v>1.392244774170681e+18</v>
       </c>
     </row>
     <row r="11">
@@ -653,20 +650,19 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hola AT_USER Quiero dejar mi voto para  el nuevo video de AT_USER dejaria todo. Gracias!💜
-#Los15Mejores #DejariaTodo #CNCO</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>Homemade fmUab</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>1.740388985762862</v>
+        <v>1.391166456168059e+18</v>
       </c>
     </row>
     <row r="12">
@@ -675,20 +671,19 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>AT_USER hola ju como andas 
-ni mal ni bien,el tuyo?</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>Madrugaciones</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1.69543289275499</v>
+        <v>1.390557884975653e+18</v>
       </c>
     </row>
     <row r="13">
@@ -697,19 +692,19 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>AT_USER hola, soy dope</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>AT_USER Pillado 🌚🤌🏻</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.737051996900189</v>
       </c>
       <c r="E13" t="n">
-        <v>1.790779697604845</v>
+        <v>1.390060154360586e+18</v>
       </c>
     </row>
     <row r="14">
@@ -718,20 +713,19 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>AT_USER Hola, AT_USER
-Para atender la solicitud y asegurar tus datos sensibles, por favor, envíanos un mens… https://t.co/LAEaPH0hmg</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
+          <t>AT_USER https://t.co/RuyG0gL9eX</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2346969914347733</v>
+        <v>1.389260722656457e+18</v>
       </c>
     </row>
     <row r="15">
@@ -740,20 +734,19 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>RT AT_USER hola oye AT_USER invita a Joaquín a cantar Black
-JOAQUIN EN LOS MTVMIAW</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>AT_USER Te dije que te callaras 👍🏻</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>-2.616621098808731</v>
       </c>
       <c r="E15" t="n">
-        <v>0.7866793330502031</v>
+        <v>1.389260171722072e+18</v>
       </c>
     </row>
     <row r="16">
@@ -762,19 +755,19 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>AT_USER hola cual es el peso permitido de su tarifa básica? Veo sus dimensiones pero el peso cual es? https://t.co/a8cby4Evxs</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>AT_USER 5€?</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.0439048163402436</v>
       </c>
       <c r="E16" t="n">
-        <v>1.252801884785093</v>
+        <v>1.388975692545724e+18</v>
       </c>
     </row>
     <row r="17">
@@ -783,20 +776,19 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>RT AT_USER Hola. Ayúdenme a llegar a los 50 seguidores para votar por Lou. Please
-Sígueme y te sigo</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>AT_USER Callate un poco</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>3.745194664102339</v>
+        <v>1.388964723392135e+18</v>
       </c>
     </row>
     <row r="18">
@@ -805,19 +797,19 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>AT_USER hola como andas???</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>Mis ojos van por caminos separados en las fotos xd</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>-1.120066456607234</v>
       </c>
       <c r="E18" t="n">
-        <v>2.440022061824547</v>
+        <v>1.388096505559622e+18</v>
       </c>
     </row>
     <row r="19">
@@ -826,19 +818,19 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>hola :)</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>No se puede salir peor</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>-1.486442344172787</v>
       </c>
       <c r="E19" t="n">
-        <v>8.300095780807117</v>
+        <v>1.388096414211838e+18</v>
       </c>
     </row>
     <row r="20">
@@ -847,19 +839,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>AT_USER hola</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
+          <t>AT_USER 🤟🏻😔🤟🏻</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>-2.211155990700567</v>
       </c>
       <c r="E20" t="n">
-        <v>1.790779697604845</v>
+        <v>1.387909008305136e+18</v>
       </c>
     </row>
     <row r="21">
@@ -868,21 +860,313 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Joel, estoy muy orgullosa de ti.
-Hola! AT_USER nomino a AT_USER para que sea host este año.
-#PremiosMTVMIAW</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="inlineStr">
+          <t>Quiero comer como un cerdo pero toca definir :(</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>-11.4775637562015</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1.387902102945534e+18</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>AT_USER el tt noseke ahjahja</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1.387495857059254e+18</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>AT_USER Hoy, no fallamos papifabri😛</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0.2643965433142731</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1.387490031603003e+18</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>El viernes orleamos✌🏻</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
         <is>
           <t>Positive</t>
         </is>
       </c>
-      <c r="E21" t="n">
-        <v>1.089865592037949</v>
+      <c r="D24" t="n">
+        <v>1.546320892343985</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1.387488811488268e+18</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>AT_USER Tremenda F</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.3615602917679208</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1.386135208244785e+18</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>A la mierda el horario 🤗</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>-2.110092760520375</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1.386126225974993e+18</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>AT_USER 🤟🏻😔🤟🏻</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>-2.211155990700567</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1.385373695812768e+18</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>AT_USER https://t.co/JqF119gaLZ</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1.38537334787838e+18</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>AT_USER Me tocara hacerte carrito en todo, nada nuevo 🤡</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>-0.2801815253279433</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.384819462327652e+18</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>AT_USER Gracias precioso 😚😚</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1.763541933749813</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.38425262739583e+18</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>A ver todas las pelis d marvel prq n tengo na mejor q hacer 🤓</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>2.593552242692311</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1.384248847325561e+18</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Y ya me ha pasao</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>1.383487764675531e+18</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Bien lo de dejar a uno de 1.60 cubrir un palo</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>-1.360775308493374</v>
+      </c>
+      <c r="E33" t="n">
+        <v>1.380966258858996e+18</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>AT_USER Dutxat porc AT_USER</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.379040941919633e+18</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Cortame mas el pelo si eso ehhhh</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0.7809984615055402</v>
+      </c>
+      <c r="E35" t="n">
+        <v>1.378427621294346e+18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Presentacion comentarios fb page
</commit_message>
<xml_diff>
--- a/Result_df/df_posts.xlsx
+++ b/Result_df/df_posts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Id</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Comments</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Id</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -481,30 +481,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>La cantante e hija de Rocío Dúrcal comparte en sus redes sociales el increíble cambio físico que ha sufrido con un método para adelgazar. Lo vemos en Corazón y tendencias
-RTVE.ES
-Shaila Dúrcal presume de cambio físico: ¡ha adelgazado 11 kilos!</t>
+          <t>GRACIAS POR ESTAR EN EL DIRECTO CON NEYMAR, NINJA Y FLAKES
+VOY PARA VER EL ÚLTIMO COMBATE
+OS QUIERO ❤️ https://t.co/IVmdUiMTdU</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.073721522464858</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2F10165091762460401</t>
-        </is>
-      </c>
+        <v>0.1213210496251103</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.397656014909026e+18</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -516,175 +514,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MGM cuenta con más de 4.000 películas en su archivo, con sagas como la de James Bond
-El anuncio se plantea en plena guerra por el control del mercado del contenido por streaming
-RTVE.ES
-Amazon compra el estudio de cine MGM</t>
+          <t>Stream con Neymar en 5 mins.
+❤️💛 https://t.co/hWQuFo0UxU https://t.co/6zdLLHwpCB</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.04812790186099442</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2F10165091728900401</t>
-        </is>
-      </c>
+        <v>0.9041762621135991</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.397624785585193e+18</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Oscar Camps, fundador de la ONG Open Arms, sobre los cadáveres aparecidos en una playa de Libia: "Llevaban tres días abandonados en la arena"
-RTVE.ES
-Aparecen en una playa de Libia los cuerpos de niños migrantes</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>-1.897418217829267</v>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2F10165091699205401</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>50</v>
-      </c>
-      <c r="I4" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Valora "dentro de la lógica de la independencia de los poderes" el informe del Tribunal Supremo, que se ha opuesto por unanimidad a conceder el indulto a los líderes del 'procés'
-RTVE.ES
-Ábalos recuerda que la decisión sobre los indultos es del Gobierno</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>-3.529292361069895</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2F10165091667095401</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>46.66666666666666</v>
-      </c>
-      <c r="H5" t="n">
-        <v>26.66666666666667</v>
-      </c>
-      <c r="I5" t="n">
-        <v>26.66666666666667</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>El streamer prepara un gran directo con enfrentamientos entre Reven vs. El Millor, Future vs. Torete y Mister Jagger vs. Viruzz.
-Te contamos todos los detalles en playz
-RTVE.ES
-Ibai Llanos: qué esperar de la velada de boxeo entre youtubers</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>-0.2689193737694566</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2F10165091625080401</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>46.66666666666666</v>
-      </c>
-      <c r="H6" t="n">
-        <v>26.66666666666667</v>
-      </c>
-      <c r="I6" t="n">
-        <v>26.66666666666667</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>La Unión Europea reclamará a AstraZeneca una compensación de "diez euros por dosis y por día de retraso" a partir del 1 de julio.
-RTVE.ES
-Bruselas reclamará a AstraZeneca 10 euros por día de retraso y dosis</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>-2.390977540065892</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2F10165091590730401</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>46.66666666666666</v>
-      </c>
-      <c r="H7" t="n">
-        <v>26.66666666666667</v>
-      </c>
-      <c r="I7" t="n">
-        <v>26.66666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>